<commit_message>
excel and json test data
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>firstName</t>
   </si>
@@ -44,6 +44,12 @@
     <t>subjects</t>
   </si>
   <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
     <t>currentAddress</t>
   </si>
   <si>
@@ -59,6 +65,12 @@
     <t>Maths</t>
   </si>
   <si>
+    <t>NCR</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
     <t>Hyderabad</t>
   </si>
   <si>
@@ -72,6 +84,12 @@
   </si>
   <si>
     <t>Physics</t>
+  </si>
+  <si>
+    <t>Rajasthan</t>
+  </si>
+  <si>
+    <t>Jaipur</t>
   </si>
   <si>
     <t>Bengaluru</t>
@@ -1227,23 +1245,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="9.72727272727273" customWidth="1"/>
     <col min="2" max="2" width="9.36363636363636" customWidth="1"/>
     <col min="3" max="3" width="14.0909090909091" customWidth="1"/>
     <col min="4" max="4" width="14.6363636363636" customWidth="1"/>
-    <col min="5" max="5" width="8.27272727272727" customWidth="1"/>
+    <col min="5" max="5" width="13.6363636363636" customWidth="1"/>
     <col min="6" max="6" width="14.9090909090909" customWidth="1"/>
+    <col min="8" max="8" width="14.9090909090909" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1262,45 +1281,63 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>9999999999</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D3">
         <v>8888888888</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>